<commit_message>
Reorganize ML section, add ability to scan geom opts (etc.) for neg freqs
</commit_message>
<xml_diff>
--- a/ligands-ML/forward_selection_MSE.xlsx
+++ b/ligands-ML/forward_selection_MSE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmwad\Desktop\repos\pd-c-photochem-ML\ligands-ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46D3D1A5-E062-4ABE-98D1-E0153E7726E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8C2D0C-97FC-419D-857B-5810A2A70EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{351659B3-5596-4067-8A3B-CD7135DC7BE6}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="LinearReg_no_agostic" sheetId="2" r:id="rId2"/>
     <sheet name="RidgeReg" sheetId="4" r:id="rId3"/>
     <sheet name="RidgeReg_no_agostic" sheetId="5" r:id="rId4"/>
+    <sheet name="default_RF_no_agostic" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="6">
   <si>
     <t>num_features</t>
   </si>
@@ -53,173 +54,17 @@
     <t>new_feature</t>
   </si>
   <si>
-    <t>Pd-H_length</t>
-  </si>
-  <si>
-    <t>vbur_far_vbur_max</t>
-  </si>
-  <si>
-    <t>vbur_far_vtot_vburminconf</t>
-  </si>
-  <si>
-    <t>sterimol_L_boltzmann_average</t>
-  </si>
-  <si>
-    <t>vmin_vmin_boltzmann_average</t>
-  </si>
-  <si>
-    <t>nbo_bd_occ_avg_boltzmann_average</t>
-  </si>
-  <si>
-    <t>vbur_ovbur_min_delta</t>
-  </si>
-  <si>
-    <t>qpoletens_yy_max</t>
-  </si>
-  <si>
-    <t>pyr_alpha_max</t>
-  </si>
-  <si>
-    <t>pyr_alpha_vburminconf</t>
-  </si>
-  <si>
-    <t>vmin_r_boltzmann_average</t>
-  </si>
-  <si>
-    <t>pyr_P_vburminconf</t>
-  </si>
-  <si>
-    <t>E_solv_total_boltzmann_average</t>
-  </si>
-  <si>
-    <t>efg_amp_P_boltzmann_average</t>
-  </si>
-  <si>
-    <t>qpole_amp_delta</t>
-  </si>
-  <si>
-    <t>spindens_P_rc_boltzmann_average</t>
-  </si>
-  <si>
-    <t>vbur_max_delta_qvtot_vburminconf</t>
-  </si>
-  <si>
-    <t>vbur_qvtot_max_min</t>
-  </si>
-  <si>
-    <t>sterimol_burB5_boltzmann_average</t>
-  </si>
-  <si>
-    <t>vbur_ovtot_max_delta</t>
-  </si>
-  <si>
-    <t>vbur_max_delta_qvbur_min</t>
-  </si>
-  <si>
-    <t>qpoletens_zz_max</t>
-  </si>
-  <si>
-    <t>vbur_qvtot_max_delta</t>
-  </si>
-  <si>
-    <t>sterimol_L_min</t>
-  </si>
-  <si>
-    <t>nbo_lp_P_percent_s_boltzmann_average</t>
-  </si>
-  <si>
-    <t>vbur_far_vtot_max</t>
-  </si>
-  <si>
     <t>alpha</t>
   </si>
   <si>
-    <t>vbur_far_vtot_boltzmann_average</t>
-  </si>
-  <si>
-    <t>vbur_far_vbur_min</t>
-  </si>
-  <si>
-    <t>qpoletens_xx_max</t>
-  </si>
-  <si>
     <t>using an arbitrary lower-limit of 1e-5 for alpha</t>
-  </si>
-  <si>
-    <t>vbur_vbur_vburminconf</t>
-  </si>
-  <si>
-    <t>vbur_ovbur_min_min</t>
-  </si>
-  <si>
-    <t>vbur_far_vbur_vburminconf</t>
-  </si>
-  <si>
-    <t>sterimol_B1_min</t>
-  </si>
-  <si>
-    <t>sterimol_burL_delta</t>
-  </si>
-  <si>
-    <t>nbo_bd_occ_min_boltzmann_average</t>
-  </si>
-  <si>
-    <t>nbo_bds_occ_avg_boltzmann_average</t>
-  </si>
-  <si>
-    <t>E_solv_elstat_boltzmann_average</t>
-  </si>
-  <si>
-    <t>nbo_bd_e_avg_boltzmann_average</t>
-  </si>
-  <si>
-    <t>qpoletens_zz_delta</t>
-  </si>
-  <si>
-    <t>nmrtens_sxx_P_boltzmann_average</t>
-  </si>
-  <si>
-    <t>sterimol_L_vburminconf</t>
-  </si>
-  <si>
-    <t>vbur_ovtot_max_boltzmann_average</t>
-  </si>
-  <si>
-    <t>sterimol_burL_vburminconf</t>
-  </si>
-  <si>
-    <t>vbur_ovbur_max_max</t>
-  </si>
-  <si>
-    <t>qpole_amp_max</t>
-  </si>
-  <si>
-    <t>vbur_ovbur_min_boltzmann_average</t>
-  </si>
-  <si>
-    <t>dipolemoment_delta</t>
-  </si>
-  <si>
-    <t>sterimol_burB5_min</t>
-  </si>
-  <si>
-    <t>efgtens_xx_P_boltzmann_average</t>
-  </si>
-  <si>
-    <t>sterimol_burL_min</t>
-  </si>
-  <si>
-    <t>sterimol_burB5_delta</t>
-  </si>
-  <si>
-    <t>qpoletens_xx_min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,13 +84,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -308,6 +146,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -329,35 +185,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,42 +385,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>69.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>62.1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>56.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>53.9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>53.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>56.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>58.9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>60.3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>56.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>59.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>65.099999999999994</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>71</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -759,6 +582,376 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>R2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>default_RF_no_agostic!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>default_RF_no_agostic!$D$2:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-24C2-4D5B-82B6-D4FD7524C398}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="375649296"/>
+        <c:axId val="375648816"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="375649296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="375648816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="375648816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="375649296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -910,42 +1103,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
-                <c:pt idx="0">
-                  <c:v>0.67400000000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.72499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.76200000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.77900000000000003</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.78900000000000003</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.79100000000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.79200000000000004</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.79400000000000004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.82</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.82099999999999995</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.82299999999999995</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.82299999999999995</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1307,54 +1464,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>170.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>123.8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>104.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>100.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>103.8</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>101.8</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>101.6</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>97.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>98.4</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>94</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>96.6</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>100.3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>99.3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>104</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1715,54 +1824,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
-                <c:pt idx="0">
-                  <c:v>0.188</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.44500000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.58399999999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.628</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.64400000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.64900000000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.68100000000000005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.70199999999999996</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.72299999999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.74</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.77</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.77800000000000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.78200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.79900000000000004</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.80100000000000005</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2120,51 +2181,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>70.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>54.8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>51.8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>49.7</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>40.700000000000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>40.5</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>39.299999999999997</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>39.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>43.6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>43.8</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>43.7</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>44.4</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>40.299999999999997</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2522,51 +2538,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>0.66800000000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.76</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.78</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.79900000000000004</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.81100000000000005</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.85599999999999998</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.86399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.873</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.877</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.877</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.877</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.877</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.878</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.88300000000000001</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.89900000000000002</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2940,66 +2911,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>170.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>123.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>104.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>96.5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>99.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>97.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>91.1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>93.2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>92.6</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90.1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>92.1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>88.5</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>84.3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>85.3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>82.8</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>81.900000000000006</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>84.4</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>84.4</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>76.2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3372,66 +3283,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
-                <c:pt idx="0">
-                  <c:v>0.188</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.443</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.58299999999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.64200000000000002</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.64700000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.67400000000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.67800000000000005</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.68600000000000005</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.70699999999999996</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.71299999999999997</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.72099999999999997</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.73</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.76800000000000002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.78300000000000003</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.78700000000000003</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.80300000000000005</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.80600000000000005</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.80600000000000005</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.81699999999999995</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.83899999999999997</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3630,7 +3481,416 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>LOOCV MSE</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>default_RF_no_agostic!$A$2:$A$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>default_RF_no_agostic!$C$2:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-63AE-4785-BB38-C98A4A288171}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="689076816"/>
+        <c:axId val="525457600"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="689076816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="525457600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="525457600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="689076816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3950,6 +4210,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4466,7 +4766,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4982,7 +5282,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5498,7 +5798,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6014,7 +6314,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6530,7 +6830,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7046,7 +7346,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7562,7 +7862,1039 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8398,6 +9730,87 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27C998FA-54D8-450C-8366-C043A6857D33}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{325EFD60-9A47-4A07-8866-7C129F742D82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8715,10 +10128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C4E1E9-851F-4BD8-A268-13F61CEBE254}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8747,169 +10160,102 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>69.7</v>
-      </c>
-      <c r="D2">
-        <v>0.67400000000000004</v>
-      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>62.1</v>
-      </c>
-      <c r="D3">
-        <v>0.72499999999999998</v>
-      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>56.4</v>
-      </c>
-      <c r="D4">
-        <v>0.76200000000000001</v>
-      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>53.9</v>
-      </c>
-      <c r="D5">
-        <v>0.77900000000000003</v>
-      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="6">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="6">
-        <v>53.5</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0.78900000000000003</v>
-      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7">
-        <v>56.2</v>
-      </c>
-      <c r="D7">
-        <v>0.79100000000000004</v>
-      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>58.9</v>
-      </c>
-      <c r="D8">
-        <v>0.79200000000000004</v>
-      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9">
-        <v>60.3</v>
-      </c>
-      <c r="D9">
-        <v>0.79400000000000004</v>
-      </c>
+      <c r="B9" s="16"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>56.5</v>
-      </c>
-      <c r="D10">
-        <v>0.82</v>
-      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11">
-        <v>59.8</v>
-      </c>
-      <c r="D11">
-        <v>0.82099999999999995</v>
-      </c>
+      <c r="B11" s="16"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12">
-        <v>65.099999999999994</v>
-      </c>
-      <c r="D12">
-        <v>0.82299999999999995</v>
-      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>71</v>
-      </c>
-      <c r="D13">
-        <v>0.82299999999999995</v>
-      </c>
+      <c r="B13" s="16"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8919,10 +10265,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98E714FB-B8ED-4E9C-BE61-ABF0CCE15C1C}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -8951,225 +10297,104 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2">
-        <v>170.5</v>
-      </c>
-      <c r="D2">
-        <v>0.188</v>
-      </c>
+      <c r="B2" s="3"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="10">
         <v>12</v>
       </c>
-      <c r="C3">
-        <v>123.8</v>
-      </c>
-      <c r="D3">
-        <v>0.44500000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>104.3</v>
-      </c>
-      <c r="D4">
-        <v>0.58399999999999996</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="6">
-        <v>100.2</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0.628</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="4">
-        <v>100.4</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.64400000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="4">
-        <v>103.8</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.64900000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4">
-        <v>101.8</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.68100000000000005</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="4">
-        <v>101.6</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.70199999999999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="4">
-        <v>97.5</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.72299999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="4">
-        <v>98.4</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="3">
-        <v>94</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="4">
-        <v>96.6</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.77800000000000002</v>
-      </c>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14">
+      <c r="A14" s="10">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="4">
-        <v>100.3</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.78200000000000003</v>
-      </c>
+      <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15">
+      <c r="A15" s="10">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="4">
-        <v>95</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.79900000000000004</v>
-      </c>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="4">
-        <v>99.3</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.8</v>
-      </c>
+      <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
+    <row r="17" spans="1:2">
+      <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="4">
-        <v>104</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.80100000000000005</v>
-      </c>
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9182,7 +10407,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9194,279 +10419,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>30</v>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>34</v>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="12">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="C2" s="12">
-        <v>70.400000000000006</v>
-      </c>
-      <c r="D2">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="E2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="12">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="12">
-        <v>54.8</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0.76</v>
-      </c>
-      <c r="E3">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="12">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="12">
-        <v>51.8</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0.78</v>
-      </c>
-      <c r="E4">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="12">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" s="12">
-        <v>50.4</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0.79900000000000004</v>
-      </c>
-      <c r="E5" s="13">
-        <v>1.0000000000000001E-5</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="12">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="12">
-        <v>49.7</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0.81100000000000005</v>
-      </c>
-      <c r="E6" s="13">
-        <v>1.0000000000000001E-5</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="8">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="8">
-        <v>40.700000000000003</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0.85599999999999998</v>
-      </c>
-      <c r="E7" s="8">
-        <v>0.01</v>
-      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="12">
-        <v>40.5</v>
-      </c>
-      <c r="D8" s="12">
-        <v>0.86399999999999999</v>
-      </c>
-      <c r="E8">
-        <v>1E-3</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="12">
-        <v>39.299999999999997</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0.873</v>
-      </c>
-      <c r="E9">
-        <v>0.01</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="12">
-        <v>39.799999999999997</v>
-      </c>
-      <c r="D10" s="12">
-        <v>0.877</v>
-      </c>
-      <c r="E10">
-        <v>0.01</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="12">
-        <v>43.2</v>
-      </c>
-      <c r="D11" s="12">
-        <v>0.877</v>
-      </c>
-      <c r="E11">
-        <v>0.01</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="12">
-        <v>43.6</v>
-      </c>
-      <c r="D12" s="12">
-        <v>0.877</v>
-      </c>
-      <c r="E12">
-        <v>0.01</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="12">
-        <v>43.8</v>
-      </c>
-      <c r="D13" s="12">
-        <v>0.877</v>
-      </c>
-      <c r="E13">
-        <v>0.01</v>
-      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="12">
-        <v>43.7</v>
-      </c>
-      <c r="D14" s="12">
-        <v>0.878</v>
-      </c>
-      <c r="E14">
-        <v>0.01</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="12">
-        <v>44.4</v>
-      </c>
-      <c r="D15" s="12">
-        <v>0.88300000000000001</v>
-      </c>
-      <c r="E15">
-        <v>0.01</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="12">
-        <v>40.299999999999997</v>
-      </c>
-      <c r="D16" s="12">
-        <v>0.89900000000000002</v>
-      </c>
-      <c r="E16">
-        <v>0.01</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9479,7 +10571,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -9491,364 +10583,363 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>30</v>
+      <c r="E1" s="10" t="s">
+        <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>34</v>
+      <c r="F1" s="10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="12">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="10"/>
+      <c r="E2" s="11"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="2"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="C2" s="12">
-        <v>170.5</v>
+      <c r="B17" s="1"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="10">
+        <v>17</v>
       </c>
-      <c r="D2">
-        <v>0.188</v>
+      <c r="B18" s="1"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="10">
+        <v>18</v>
       </c>
-      <c r="E2" s="13">
-        <v>1.0000000000000001E-5</v>
+      <c r="B19" s="1"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="10">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5EFAC3-79CD-4473-B682-B3E361B8B529}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="12">
+    <row r="2" spans="1:4">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="12">
-        <v>123.5</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0.443</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="12">
+    <row r="4" spans="1:4">
+      <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="12">
-        <v>104.3</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="E4">
-        <v>0.1</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="12">
+    <row r="5" spans="1:4">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="12">
-        <v>96.5</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0.64200000000000002</v>
-      </c>
-      <c r="E5" s="13">
-        <v>0.1</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="12">
+    <row r="6" spans="1:4">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="12">
-        <v>99.2</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0.64700000000000002</v>
-      </c>
-      <c r="E6" s="13">
-        <v>1.0000000000000001E-5</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="12">
+    <row r="7" spans="1:4">
+      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="12">
-        <v>97.2</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0.67400000000000004</v>
-      </c>
-      <c r="E7" s="15">
-        <v>1.0000000000000001E-5</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="8">
+    <row r="8" spans="1:4">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="8">
-        <v>91.1</v>
-      </c>
-      <c r="D8" s="8">
-        <v>0.67800000000000005</v>
-      </c>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="12">
-        <v>93.2</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0.68600000000000005</v>
-      </c>
-      <c r="E9">
-        <v>0.1</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="12">
-        <v>92.6</v>
-      </c>
-      <c r="D10" s="12">
-        <v>0.70699999999999996</v>
-      </c>
-      <c r="E10">
-        <v>0.1</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="12">
-        <v>90.1</v>
-      </c>
-      <c r="D11" s="12">
-        <v>0.71299999999999997</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="12">
-        <v>91</v>
-      </c>
-      <c r="D12" s="12">
-        <v>0.72099999999999997</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="12">
-        <v>92.1</v>
-      </c>
-      <c r="D13" s="12">
-        <v>0.73</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="4">
+    <row r="14" spans="1:4">
+      <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="12">
-        <v>88.5</v>
-      </c>
-      <c r="D14" s="12">
-        <v>0.76800000000000002</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="3">
+    <row r="15" spans="1:4">
+      <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="14">
-        <v>84.3</v>
-      </c>
-      <c r="D15" s="14">
-        <v>0.78300000000000003</v>
-      </c>
-      <c r="E15" s="3">
-        <v>1</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C16" s="12">
-        <v>85.3</v>
-      </c>
-      <c r="D16" s="12">
-        <v>0.78700000000000003</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="12">
-        <v>82.8</v>
-      </c>
-      <c r="D17" s="12">
-        <v>0.80300000000000005</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="12">
-        <v>81.900000000000006</v>
-      </c>
-      <c r="D18" s="12">
-        <v>0.80600000000000005</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" s="12">
-        <v>84.4</v>
-      </c>
-      <c r="D19" s="12">
-        <v>0.80600000000000005</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C20" s="12">
-        <v>84.4</v>
-      </c>
-      <c r="D20" s="12">
-        <v>0.81699999999999995</v>
-      </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:5">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="12">
-        <v>76.2</v>
-      </c>
-      <c r="D21" s="12">
-        <v>0.83899999999999997</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
+    <row r="22" spans="1:3">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="B23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>